<commit_message>
Added a gamma test result at 10V (both pumps)
</commit_message>
<xml_diff>
--- a/Tanques quádruplos - Identificação/Data/Gamma1e2.xlsx
+++ b/Tanques quádruplos - Identificação/Data/Gamma1e2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Tanques</t>
   </si>
@@ -376,10 +376,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,6 +472,90 @@
         <v>6.8</v>
       </c>
     </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" s="1">
+        <v>5.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="1">
+        <v>16.2</v>
+      </c>
+      <c r="C14" s="1">
+        <v>16</v>
+      </c>
+      <c r="E14">
+        <f>B14/(B14+B17)</f>
+        <v>0.6206896551724137</v>
+      </c>
+      <c r="F14">
+        <f>B15/(B15+B16)</f>
+        <v>0.59469696969696972</v>
+      </c>
+      <c r="G14">
+        <f>E14+F14</f>
+        <v>1.2153866248693834</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15" s="1">
+        <v>15.7</v>
+      </c>
+      <c r="C15" s="1">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1">
+        <v>10.7</v>
+      </c>
+      <c r="C16" s="1">
+        <v>6.6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1">
+        <v>9.9</v>
+      </c>
+      <c r="C17" s="1">
+        <v>6.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>